<commit_message>
calibrated all sensors and added new 2 point interpolation code
</commit_message>
<xml_diff>
--- a/QtClients/TargetLocatorSensorData/CalibrationData.xlsx
+++ b/QtClients/TargetLocatorSensorData/CalibrationData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9510" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9510" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Top Left IR Sensor" sheetId="3" r:id="rId2"/>
-    <sheet name="Top Right IR Sensor" sheetId="4" r:id="rId3"/>
+    <sheet name="Bottom Left LR" sheetId="1" r:id="rId1"/>
+    <sheet name="Bottom Right LR" sheetId="5" r:id="rId2"/>
+    <sheet name="Top Left LR" sheetId="6" r:id="rId3"/>
+    <sheet name="Top Right LR" sheetId="7" r:id="rId4"/>
+    <sheet name="Middle MR" sheetId="8" r:id="rId5"/>
+    <sheet name="Left MR" sheetId="9" r:id="rId6"/>
+    <sheet name="Right MR" sheetId="10" r:id="rId7"/>
+    <sheet name="Top Left IR Sensor.bak" sheetId="3" r:id="rId8"/>
+    <sheet name="Top Right IR Sensor.bak" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="5">
   <si>
     <t>Distance</t>
   </si>
@@ -163,36 +169,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -204,396 +180,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Inverse Distance</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$15</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.3333333333333333E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6666666666666666E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.4285714285714285E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.2500000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.1111111111111112E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.0909090909090905E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.3333333333333332E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7.6923076923076927E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7.1428571428571426E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.6666666666666671E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>2.5099999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.52</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.06</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.93</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.72499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.47499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.45</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7F80-468C-B516-4B8339CC657D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="397973648"/>
-        <c:axId val="397972336"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="397973648"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="397972336"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="397972336"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="397973648"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Top Left IR Sensor'!$C$1</c:f>
+              <c:f>'Top Left IR Sensor.bak'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -676,7 +263,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Top Left IR Sensor'!$C$2:$C$10</c:f>
+              <c:f>'Top Left IR Sensor.bak'!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -712,7 +299,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Top Left IR Sensor'!$B$2:$B$10</c:f>
+              <c:f>'Top Left IR Sensor.bak'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -833,7 +420,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Top Left IR Sensor'!$C$10:$C$13</c:f>
+              <c:f>'Top Left IR Sensor.bak'!$C$10:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -854,7 +441,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Top Left IR Sensor'!$B$10:$B$13</c:f>
+              <c:f>'Top Left IR Sensor.bak'!$B$10:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1074,7 +661,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1099,7 +686,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Top Right IR Sensor'!$C$1</c:f>
+              <c:f>'Top Right IR Sensor.bak'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1182,7 +769,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Top Right IR Sensor'!$C$2:$C$10</c:f>
+              <c:f>'Top Right IR Sensor.bak'!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1218,7 +805,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Top Right IR Sensor'!$B$2:$B$10</c:f>
+              <c:f>'Top Right IR Sensor.bak'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1339,7 +926,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Top Right IR Sensor'!$C$10:$C$13</c:f>
+              <c:f>'Top Right IR Sensor.bak'!$C$10:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1360,7 +947,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Top Right IR Sensor'!$B$10:$B$13</c:f>
+              <c:f>'Top Right IR Sensor.bak'!$B$10:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1660,46 +1247,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2732,564 +2279,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>490537</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>185737</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3332,20 +2322,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>80401</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>169769</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>302559</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>118124</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>113739</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>169769</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>526396</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>73788</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3676,20 +2666,17 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3697,182 +2684,985 @@
         <v>20</v>
       </c>
       <c r="B2" s="1">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="C2" s="4">
-        <f>1/A2</f>
-        <v>0.05</v>
-      </c>
+        <v>2.508</v>
+      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4">
-        <f t="shared" ref="C3:C15" si="0">1/A3</f>
-        <v>3.3333333333333333E-2</v>
+        <v>2.2130000000000001</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B2-B3</f>
+        <v>0.29499999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>40</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1.52</v>
-      </c>
-      <c r="C4" s="4">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <v>30</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.881</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C12" si="0">B3-B4</f>
+        <v>0.33200000000000007</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="C5" s="4">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>1.621</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1">
-        <v>1.06</v>
-      </c>
-      <c r="C6" s="4">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666666E-2</v>
+        <v>1.415</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.20599999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1">
-        <v>0.93</v>
-      </c>
-      <c r="C7" s="4">
-        <f t="shared" si="0"/>
-        <v>1.4285714285714285E-2</v>
+        <v>1.2450000000000001</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.16999999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="0"/>
-        <v>1.2500000000000001E-2</v>
+        <v>1.113</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.13200000000000012</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="0"/>
-        <v>1.1111111111111112E-2</v>
+        <v>1.0069999999999999</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10600000000000009</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1">
-        <v>0.65</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>8.4999999999999853E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="0"/>
-        <v>9.0909090909090905E-3</v>
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>8.1000000000000072E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="C12" s="4">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333332E-3</v>
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999942E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>130</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C13" s="4">
-        <f t="shared" si="0"/>
-        <v>7.6923076923076927E-3</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>140</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="C14" s="4">
-        <f t="shared" si="0"/>
-        <v>7.1428571428571426E-3</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>150</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="C15" s="4">
-        <f t="shared" si="0"/>
-        <v>6.6666666666666671E-3</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="A1:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2.4300000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.1269999999999998</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B2-B3</f>
+        <v>0.30300000000000038</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.8540000000000001</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C12" si="0">B3-B4</f>
+        <v>0.27299999999999969</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.5880000000000001</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.387</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.20100000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.2190000000000001</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.16799999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>50</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>55</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1180000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>9.8999999999999977E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>65</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>7.6999999999999957E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>70</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000064E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2.5350000000000001</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.2330000000000001</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B2-B3</f>
+        <v>0.30200000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.9410000000000001</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C12" si="0">B3-B4</f>
+        <v>0.29200000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.6830000000000001</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.25800000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.4790000000000001</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.20399999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.3180000000000001</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.16100000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>50</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.173</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.14500000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>55</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10600000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10399999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>65</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>7.3999999999999955E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>70</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>5.1000000000000045E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.2210000000000001</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B2-B3</f>
+        <v>0.2889999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.948</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C12" si="0">B3-B4</f>
+        <v>0.27300000000000013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.6879999999999999</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.4890000000000001</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.19899999999999984</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.33</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.15900000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>50</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.2110000000000001</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>55</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1.099</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1120000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>9.8000000000000087E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>65</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>7.0999999999999841E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>70</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>6.5000000000000058E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="A2:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3.0510000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.3119999999999998</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B2-B3</f>
+        <v>0.73900000000000032</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C9" si="0">B3-B4</f>
+        <v>0.71199999999999974</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.232</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3680000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.15600000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>35</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>9.3999999999999972E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>40</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>8.3999999999999964E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3.048</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.3010000000000002</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B2-B3</f>
+        <v>0.74699999999999989</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.5620000000000001</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C9" si="0">B3-B4</f>
+        <v>0.7390000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.2130000000000001</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.34899999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.23000000000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.14100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>35</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>40</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>6.6999999999999948E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2.9590000000000001</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.218</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B2-B3</f>
+        <v>0.7410000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.569</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C9" si="0">B3-B4</f>
+        <v>0.64900000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.2210000000000001</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.34799999999999986</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.23000000000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.15800000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>35</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10299999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>40</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>8.5999999999999965E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4177,13 +3967,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J179"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>